<commit_message>
finalizacao dos documentos e relatorio da sprint3
</commit_message>
<xml_diff>
--- a/documentos/sprint-3/Template_Matriz das Comunicacoes.xlsx
+++ b/documentos/sprint-3/Template_Matriz das Comunicacoes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="123820"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erica Santos\Desktop\6º Semestre\Gestão de Projetos\07-Gerenciamento de Comunicação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erica Santos\Desktop\6º Semestre\Gestão de Projetos\sprint-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2855B690-17F2-4586-B444-F6E25DD010CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E9C1B3-2301-44BA-9BE4-6EB16A85E229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="130">
   <si>
     <t>Matriz das comunicações</t>
   </si>
@@ -453,7 +453,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -701,12 +701,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1308,7 +1302,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1467,74 +1461,16 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="21" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="21" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="20" fillId="39" borderId="18" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="39" borderId="19" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="39" borderId="20" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="45" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="21" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="22" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="24" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="32" fillId="40" borderId="1" xfId="44" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="38" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="38" borderId="17" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="12" borderId="18" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="12" borderId="19" xfId="1" applyBorder="1" applyAlignment="1"/>
@@ -1542,25 +1478,80 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="38" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="38" borderId="1" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="38" borderId="17" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="21" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="22" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="39" borderId="18" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="39" borderId="19" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="39" borderId="20" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="45" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="24" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="21" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="21" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="12" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="40" borderId="1" xfId="44" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="40" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -2165,17 +2156,17 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:11" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="99"/>
-      <c r="J11" s="99"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
     </row>
     <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="51" t="s">
@@ -2187,50 +2178,50 @@
       <c r="D12" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="101" t="s">
+      <c r="E12" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="101"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="101"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="101"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
     </row>
     <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="52"/>
       <c r="C13" s="52"/>
       <c r="D13" s="55"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
     </row>
     <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="52"/>
       <c r="C14" s="52"/>
       <c r="D14" s="55"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="102"/>
-      <c r="J14" s="102"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
     </row>
     <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:11" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="103" t="s">
+      <c r="B16" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="103"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="103"/>
-      <c r="F16" s="103"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="103"/>
-      <c r="I16" s="103"/>
-      <c r="J16" s="103"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
     </row>
     <row r="17" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="51" t="s">
@@ -2242,14 +2233,14 @@
       <c r="D17" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="93" t="s">
+      <c r="E17" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="94"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="94"/>
-      <c r="J17" s="95"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="73"/>
     </row>
     <row r="18" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="52">
@@ -2257,12 +2248,12 @@
       </c>
       <c r="C18" s="52"/>
       <c r="D18" s="55"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="97"/>
-      <c r="G18" s="97"/>
-      <c r="H18" s="97"/>
-      <c r="I18" s="97"/>
-      <c r="J18" s="98"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="76"/>
     </row>
     <row r="19" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="52">
@@ -2270,26 +2261,26 @@
       </c>
       <c r="C19" s="52"/>
       <c r="D19" s="55"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="97"/>
-      <c r="G19" s="97"/>
-      <c r="H19" s="97"/>
-      <c r="I19" s="97"/>
-      <c r="J19" s="98"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="76"/>
     </row>
     <row r="20" spans="2:10" ht="15.6" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:10" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="99" t="s">
+      <c r="B21" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="99"/>
-      <c r="D21" s="99"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="99"/>
-      <c r="I21" s="99"/>
-      <c r="J21" s="99"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
     </row>
     <row r="22" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="56" t="s">
@@ -2301,14 +2292,14 @@
       <c r="D22" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="100" t="s">
+      <c r="E22" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="100"/>
-      <c r="G22" s="100"/>
-      <c r="H22" s="100"/>
-      <c r="I22" s="100"/>
-      <c r="J22" s="100"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="77"/>
     </row>
     <row r="23" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="55">
@@ -2318,14 +2309,14 @@
         <v>21</v>
       </c>
       <c r="D23" s="55"/>
-      <c r="E23" s="91" t="s">
+      <c r="E23" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="91"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="91"/>
-      <c r="I23" s="91"/>
-      <c r="J23" s="91"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="78"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="55" t="s">
@@ -2335,14 +2326,14 @@
         <v>21</v>
       </c>
       <c r="D24" s="55"/>
-      <c r="E24" s="91" t="s">
+      <c r="E24" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="91"/>
-      <c r="G24" s="91"/>
-      <c r="H24" s="91"/>
-      <c r="I24" s="91"/>
-      <c r="J24" s="91"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="78"/>
+      <c r="J24" s="78"/>
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="55" t="s">
@@ -2352,14 +2343,14 @@
         <v>21</v>
       </c>
       <c r="D25" s="55"/>
-      <c r="E25" s="91" t="s">
+      <c r="E25" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="91"/>
-      <c r="I25" s="91"/>
-      <c r="J25" s="91"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="55" t="s">
@@ -2369,14 +2360,14 @@
         <v>21</v>
       </c>
       <c r="D26" s="55"/>
-      <c r="E26" s="91" t="s">
+      <c r="E26" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="91"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="91"/>
-      <c r="I26" s="91"/>
-      <c r="J26" s="91"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="55">
@@ -2386,14 +2377,14 @@
         <v>21</v>
       </c>
       <c r="D27" s="55"/>
-      <c r="E27" s="91" t="s">
+      <c r="E27" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="91"/>
-      <c r="G27" s="91"/>
-      <c r="H27" s="91"/>
-      <c r="I27" s="91"/>
-      <c r="J27" s="91"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="78"/>
+      <c r="J27" s="78"/>
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="55" t="s">
@@ -2403,14 +2394,14 @@
         <v>31</v>
       </c>
       <c r="D28" s="55"/>
-      <c r="E28" s="91" t="s">
+      <c r="E28" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="91"/>
-      <c r="G28" s="91"/>
-      <c r="H28" s="91"/>
-      <c r="I28" s="91"/>
-      <c r="J28" s="91"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="78"/>
+      <c r="J28" s="78"/>
     </row>
     <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="55" t="s">
@@ -2420,14 +2411,14 @@
         <v>21</v>
       </c>
       <c r="D29" s="55"/>
-      <c r="E29" s="91" t="s">
+      <c r="E29" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="91"/>
-      <c r="G29" s="91"/>
-      <c r="H29" s="91"/>
-      <c r="I29" s="91"/>
-      <c r="J29" s="91"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="78"/>
+      <c r="J29" s="78"/>
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="55" t="s">
@@ -2437,253 +2428,228 @@
         <v>21</v>
       </c>
       <c r="D30" s="55"/>
-      <c r="E30" s="91" t="s">
+      <c r="E30" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="91"/>
-      <c r="G30" s="91"/>
-      <c r="H30" s="91"/>
-      <c r="I30" s="91"/>
-      <c r="J30" s="91"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="78"/>
+      <c r="J30" s="78"/>
     </row>
     <row r="31" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="53"/>
       <c r="C31" s="54"/>
       <c r="D31" s="53"/>
-      <c r="E31" s="92"/>
-      <c r="F31" s="92"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="92"/>
-      <c r="I31" s="92"/>
-      <c r="J31" s="92"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="79"/>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="85" t="s">
+      <c r="B32" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="86"/>
-      <c r="H32" s="86"/>
-      <c r="I32" s="86"/>
-      <c r="J32" s="87"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="81"/>
+      <c r="G32" s="81"/>
+      <c r="H32" s="81"/>
+      <c r="I32" s="81"/>
+      <c r="J32" s="82"/>
     </row>
     <row r="33" spans="2:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="82"/>
-      <c r="D33" s="82"/>
-      <c r="E33" s="82"/>
-      <c r="F33" s="82"/>
-      <c r="G33" s="82"/>
-      <c r="H33" s="82"/>
-      <c r="I33" s="82"/>
-      <c r="J33" s="83"/>
+      <c r="C33" s="84"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="84"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="84"/>
+      <c r="J33" s="85"/>
     </row>
     <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="84"/>
-      <c r="C34" s="84"/>
-      <c r="D34" s="84"/>
-      <c r="E34" s="84"/>
-      <c r="F34" s="84"/>
-      <c r="G34" s="84"/>
-      <c r="H34" s="84"/>
-      <c r="I34" s="84"/>
-      <c r="J34" s="84"/>
+      <c r="B34" s="86"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="86"/>
+      <c r="H34" s="86"/>
+      <c r="I34" s="86"/>
+      <c r="J34" s="86"/>
     </row>
     <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="85" t="s">
+      <c r="B35" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="86"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
-      <c r="J35" s="87"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="81"/>
+      <c r="G35" s="81"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="82"/>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="88" t="s">
+      <c r="B36" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="89"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="89"/>
-      <c r="G36" s="89"/>
-      <c r="H36" s="89"/>
-      <c r="I36" s="89"/>
-      <c r="J36" s="90"/>
+      <c r="C36" s="88"/>
+      <c r="D36" s="88"/>
+      <c r="E36" s="88"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="88"/>
+      <c r="H36" s="88"/>
+      <c r="I36" s="88"/>
+      <c r="J36" s="89"/>
     </row>
     <row r="37" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="78" t="s">
+      <c r="B37" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="79"/>
-      <c r="D37" s="79"/>
-      <c r="E37" s="79"/>
-      <c r="F37" s="79"/>
-      <c r="G37" s="79"/>
-      <c r="H37" s="79"/>
-      <c r="I37" s="79"/>
-      <c r="J37" s="80"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="91"/>
+      <c r="E37" s="91"/>
+      <c r="F37" s="91"/>
+      <c r="G37" s="91"/>
+      <c r="H37" s="91"/>
+      <c r="I37" s="91"/>
+      <c r="J37" s="92"/>
     </row>
     <row r="38" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="66"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="67"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="H38" s="67"/>
-      <c r="I38" s="67"/>
-      <c r="J38" s="68"/>
+      <c r="B38" s="93"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="94"/>
+      <c r="G38" s="94"/>
+      <c r="H38" s="94"/>
+      <c r="I38" s="94"/>
+      <c r="J38" s="95"/>
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="69" t="s">
+      <c r="B39" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="70"/>
-      <c r="D39" s="70"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="70"/>
-      <c r="H39" s="70"/>
-      <c r="I39" s="70"/>
-      <c r="J39" s="71"/>
+      <c r="C39" s="97"/>
+      <c r="D39" s="97"/>
+      <c r="E39" s="97"/>
+      <c r="F39" s="97"/>
+      <c r="G39" s="97"/>
+      <c r="H39" s="97"/>
+      <c r="I39" s="97"/>
+      <c r="J39" s="98"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="69" t="s">
+      <c r="B40" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="70"/>
-      <c r="D40" s="70"/>
-      <c r="E40" s="70"/>
-      <c r="F40" s="70"/>
-      <c r="G40" s="70"/>
-      <c r="H40" s="70"/>
-      <c r="I40" s="70"/>
-      <c r="J40" s="71"/>
+      <c r="C40" s="97"/>
+      <c r="D40" s="97"/>
+      <c r="E40" s="97"/>
+      <c r="F40" s="97"/>
+      <c r="G40" s="97"/>
+      <c r="H40" s="97"/>
+      <c r="I40" s="97"/>
+      <c r="J40" s="98"/>
     </row>
     <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="70"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="71"/>
+      <c r="C41" s="97"/>
+      <c r="D41" s="97"/>
+      <c r="E41" s="97"/>
+      <c r="F41" s="97"/>
+      <c r="G41" s="97"/>
+      <c r="H41" s="97"/>
+      <c r="I41" s="97"/>
+      <c r="J41" s="98"/>
     </row>
     <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="75"/>
-      <c r="C42" s="76"/>
-      <c r="D42" s="76"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="76"/>
-      <c r="G42" s="76"/>
-      <c r="H42" s="76"/>
-      <c r="I42" s="76"/>
-      <c r="J42" s="77"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="103"/>
+      <c r="D42" s="103"/>
+      <c r="E42" s="103"/>
+      <c r="F42" s="103"/>
+      <c r="G42" s="103"/>
+      <c r="H42" s="103"/>
+      <c r="I42" s="103"/>
+      <c r="J42" s="104"/>
     </row>
     <row r="43" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="78" t="s">
+      <c r="B43" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="79"/>
-      <c r="D43" s="79"/>
-      <c r="E43" s="79"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="79"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="79"/>
-      <c r="J43" s="80"/>
+      <c r="C43" s="91"/>
+      <c r="D43" s="91"/>
+      <c r="E43" s="91"/>
+      <c r="F43" s="91"/>
+      <c r="G43" s="91"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="91"/>
+      <c r="J43" s="92"/>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="69" t="s">
+      <c r="B44" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="70"/>
-      <c r="H44" s="70"/>
-      <c r="I44" s="70"/>
-      <c r="J44" s="71"/>
+      <c r="C44" s="97"/>
+      <c r="D44" s="97"/>
+      <c r="E44" s="97"/>
+      <c r="F44" s="97"/>
+      <c r="G44" s="97"/>
+      <c r="H44" s="97"/>
+      <c r="I44" s="97"/>
+      <c r="J44" s="98"/>
     </row>
     <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="69" t="s">
+      <c r="B45" s="96" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="70"/>
-      <c r="D45" s="70"/>
-      <c r="E45" s="70"/>
-      <c r="F45" s="70"/>
-      <c r="G45" s="70"/>
-      <c r="H45" s="70"/>
-      <c r="I45" s="70"/>
-      <c r="J45" s="71"/>
+      <c r="C45" s="97"/>
+      <c r="D45" s="97"/>
+      <c r="E45" s="97"/>
+      <c r="F45" s="97"/>
+      <c r="G45" s="97"/>
+      <c r="H45" s="97"/>
+      <c r="I45" s="97"/>
+      <c r="J45" s="98"/>
     </row>
     <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="69" t="s">
+      <c r="B46" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="70"/>
-      <c r="D46" s="70"/>
-      <c r="E46" s="70"/>
-      <c r="F46" s="70"/>
-      <c r="G46" s="70"/>
-      <c r="H46" s="70"/>
-      <c r="I46" s="70"/>
-      <c r="J46" s="71"/>
+      <c r="C46" s="97"/>
+      <c r="D46" s="97"/>
+      <c r="E46" s="97"/>
+      <c r="F46" s="97"/>
+      <c r="G46" s="97"/>
+      <c r="H46" s="97"/>
+      <c r="I46" s="97"/>
+      <c r="J46" s="98"/>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="72"/>
-      <c r="C47" s="73"/>
-      <c r="D47" s="73"/>
-      <c r="E47" s="73"/>
-      <c r="F47" s="73"/>
-      <c r="G47" s="73"/>
-      <c r="H47" s="73"/>
-      <c r="I47" s="73"/>
-      <c r="J47" s="74"/>
+      <c r="B47" s="99"/>
+      <c r="C47" s="100"/>
+      <c r="D47" s="100"/>
+      <c r="E47" s="100"/>
+      <c r="F47" s="100"/>
+      <c r="G47" s="100"/>
+      <c r="H47" s="100"/>
+      <c r="I47" s="100"/>
+      <c r="J47" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="B32:J32"/>
-    <mergeCell ref="B33:J33"/>
-    <mergeCell ref="B34:J34"/>
-    <mergeCell ref="B35:J35"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="B37:J37"/>
     <mergeCell ref="B38:J38"/>
     <mergeCell ref="B39:J39"/>
     <mergeCell ref="B40:J40"/>
@@ -2694,6 +2660,31 @@
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
     <mergeCell ref="B46:J46"/>
+    <mergeCell ref="B33:J33"/>
+    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="B32:J32"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="B16:J16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D5" location="Informacoes!A1" display="Informações" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2733,10 +2724,10 @@
   <dimension ref="B1:P9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2762,12 +2753,12 @@
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="104" t="s">
+      <c r="E2" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
       <c r="I2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -2846,9 +2837,7 @@
       <c r="L4" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" spans="2:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
@@ -2991,7 +2980,7 @@
       <c r="J8" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="K8" s="105" t="s">
+      <c r="K8" s="66" t="s">
         <v>129</v>
       </c>
       <c r="L8" s="59" t="s">
@@ -3029,7 +3018,7 @@
       <c r="J9" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="K9" s="106" t="s">
+      <c r="K9" s="66" t="s">
         <v>111</v>
       </c>
       <c r="L9" s="59" t="s">
@@ -3097,12 +3086,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E1" s="104" t="s">
+      <c r="E1" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
     </row>
     <row r="2" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
@@ -3358,21 +3347,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F03B8E1887DC68468EE864D08E963882" ma:contentTypeVersion="7" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="91b20acb9f322c1796d6f7b010a9821c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="426a5322-44b7-4b51-acaa-2bde68eff610" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20a2a9ead06364c8482e0559047a30aa" ns2:_="">
     <xsd:import namespace="426a5322-44b7-4b51-acaa-2bde68eff610"/>
@@ -3536,24 +3510,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F023C16-AACF-4D0D-B071-9C130BD3ABA5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D646DE-231A-42E1-9347-E7CB0B60D08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B8388F-8728-4BD2-A83F-F4F966F2B0F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3569,4 +3541,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D646DE-231A-42E1-9347-E7CB0B60D08E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F023C16-AACF-4D0D-B071-9C130BD3ABA5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>